<commit_message>
revision of source codes
</commit_message>
<xml_diff>
--- a/results/artifacts/df_weight_sensitivity_150_fig8.xlsx
+++ b/results/artifacts/df_weight_sensitivity_150_fig8.xlsx
@@ -517,7 +517,7 @@
         <v>0.01</v>
       </c>
       <c r="F2" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G2" t="n">
         <v>0.25</v>
@@ -535,7 +535,7 @@
         <v>12.09</v>
       </c>
       <c r="L2" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M2" t="n">
         <v>97</v>
@@ -561,7 +561,7 @@
         <v>0.01</v>
       </c>
       <c r="F3" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G3" t="n">
         <v>0.25</v>
@@ -579,7 +579,7 @@
         <v>12.09</v>
       </c>
       <c r="L3" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M3" t="n">
         <v>97</v>
@@ -605,7 +605,7 @@
         <v>0.25</v>
       </c>
       <c r="F4" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G4" t="n">
         <v>0.25</v>
@@ -623,7 +623,7 @@
         <v>10.66</v>
       </c>
       <c r="L4" t="n">
-        <v>7069724.04</v>
+        <v>825974.04</v>
       </c>
       <c r="M4" t="n">
         <v>90</v>
@@ -649,7 +649,7 @@
         <v>0.25</v>
       </c>
       <c r="F5" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G5" t="n">
         <v>0.25</v>
@@ -667,7 +667,7 @@
         <v>10.66</v>
       </c>
       <c r="L5" t="n">
-        <v>19569724.04</v>
+        <v>7069724.04</v>
       </c>
       <c r="M5" t="n">
         <v>90</v>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G6" t="n">
         <v>0.25</v>
@@ -711,7 +711,7 @@
         <v>7.24</v>
       </c>
       <c r="L6" t="n">
-        <v>8819721.039999999</v>
+        <v>827721.04</v>
       </c>
       <c r="M6" t="n">
         <v>78</v>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G7" t="n">
         <v>0.25</v>
@@ -755,7 +755,7 @@
         <v>7.24</v>
       </c>
       <c r="L7" t="n">
-        <v>24819721.04</v>
+        <v>8819721.039999999</v>
       </c>
       <c r="M7" t="n">
         <v>78</v>
@@ -781,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G8" t="n">
         <v>0.25</v>
@@ -799,7 +799,7 @@
         <v>-4.07</v>
       </c>
       <c r="L8" t="n">
-        <v>9319720.289999999</v>
+        <v>828220.29</v>
       </c>
       <c r="M8" t="n">
         <v>32</v>
@@ -825,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G9" t="n">
         <v>0.25</v>
@@ -843,7 +843,7 @@
         <v>-4.07</v>
       </c>
       <c r="L9" t="n">
-        <v>26319720.29</v>
+        <v>9319720.289999999</v>
       </c>
       <c r="M9" t="n">
         <v>32</v>
@@ -869,7 +869,7 @@
         <v>100</v>
       </c>
       <c r="F10" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G10" t="n">
         <v>0.25</v>
@@ -887,7 +887,7 @@
         <v>-75.31</v>
       </c>
       <c r="L10" t="n">
-        <v>9319720.289999999</v>
+        <v>828220.29</v>
       </c>
       <c r="M10" t="n">
         <v>28</v>
@@ -913,7 +913,7 @@
         <v>100</v>
       </c>
       <c r="F11" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G11" t="n">
         <v>0.25</v>
@@ -931,7 +931,7 @@
         <v>-75.31</v>
       </c>
       <c r="L11" t="n">
-        <v>26319720.29</v>
+        <v>9319720.289999999</v>
       </c>
       <c r="M11" t="n">
         <v>28</v>
@@ -957,7 +957,7 @@
         <v>0.01</v>
       </c>
       <c r="F12" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G12" t="n">
         <v>0.25</v>
@@ -975,7 +975,7 @@
         <v>23.03</v>
       </c>
       <c r="L12" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M12" t="n">
         <v>97</v>
@@ -1001,7 +1001,7 @@
         <v>0.01</v>
       </c>
       <c r="F13" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G13" t="n">
         <v>0.25</v>
@@ -1019,7 +1019,7 @@
         <v>23.03</v>
       </c>
       <c r="L13" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M13" t="n">
         <v>97</v>
@@ -1045,7 +1045,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G14" t="n">
         <v>0.25</v>
@@ -1063,7 +1063,7 @@
         <v>21.56</v>
       </c>
       <c r="L14" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M14" t="n">
         <v>97</v>
@@ -1089,7 +1089,7 @@
         <v>0.25</v>
       </c>
       <c r="F15" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G15" t="n">
         <v>0.25</v>
@@ -1107,7 +1107,7 @@
         <v>21.56</v>
       </c>
       <c r="L15" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M15" t="n">
         <v>97</v>
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G16" t="n">
         <v>0.25</v>
@@ -1151,7 +1151,7 @@
         <v>17.23</v>
       </c>
       <c r="L16" t="n">
-        <v>8569724.789999999</v>
+        <v>827474.79</v>
       </c>
       <c r="M16" t="n">
         <v>89</v>
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G17" t="n">
         <v>0.25</v>
@@ -1195,7 +1195,7 @@
         <v>17.23</v>
       </c>
       <c r="L17" t="n">
-        <v>24069724.79</v>
+        <v>8569724.789999999</v>
       </c>
       <c r="M17" t="n">
         <v>89</v>
@@ -1221,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="F18" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G18" t="n">
         <v>0.25</v>
@@ -1239,7 +1239,7 @@
         <v>1.95</v>
       </c>
       <c r="L18" t="n">
-        <v>9319720.289999999</v>
+        <v>828220.29</v>
       </c>
       <c r="M18" t="n">
         <v>33</v>
@@ -1265,7 +1265,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G19" t="n">
         <v>0.25</v>
@@ -1283,7 +1283,7 @@
         <v>1.95</v>
       </c>
       <c r="L19" t="n">
-        <v>26319720.29</v>
+        <v>9319720.289999999</v>
       </c>
       <c r="M19" t="n">
         <v>33</v>
@@ -1309,7 +1309,7 @@
         <v>100</v>
       </c>
       <c r="F20" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G20" t="n">
         <v>0.25</v>
@@ -1327,7 +1327,7 @@
         <v>-69.72</v>
       </c>
       <c r="L20" t="n">
-        <v>9319720.289999999</v>
+        <v>828220.29</v>
       </c>
       <c r="M20" t="n">
         <v>28</v>
@@ -1353,7 +1353,7 @@
         <v>100</v>
       </c>
       <c r="F21" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G21" t="n">
         <v>0.25</v>
@@ -1371,7 +1371,7 @@
         <v>-69.72</v>
       </c>
       <c r="L21" t="n">
-        <v>26319720.29</v>
+        <v>9319720.289999999</v>
       </c>
       <c r="M21" t="n">
         <v>28</v>
@@ -1397,7 +1397,7 @@
         <v>0.01</v>
       </c>
       <c r="F22" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G22" t="n">
         <v>0.25</v>
@@ -1415,7 +1415,7 @@
         <v>467.2</v>
       </c>
       <c r="L22" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M22" t="n">
         <v>96</v>
@@ -1441,7 +1441,7 @@
         <v>0.01</v>
       </c>
       <c r="F23" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G23" t="n">
         <v>0.25</v>
@@ -1459,7 +1459,7 @@
         <v>467.2</v>
       </c>
       <c r="L23" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M23" t="n">
         <v>96</v>
@@ -1485,7 +1485,7 @@
         <v>0.25</v>
       </c>
       <c r="F24" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G24" t="n">
         <v>0.25</v>
@@ -1503,7 +1503,7 @@
         <v>465.76</v>
       </c>
       <c r="L24" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M24" t="n">
         <v>96</v>
@@ -1529,7 +1529,7 @@
         <v>0.25</v>
       </c>
       <c r="F25" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G25" t="n">
         <v>0.25</v>
@@ -1547,7 +1547,7 @@
         <v>465.76</v>
       </c>
       <c r="L25" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M25" t="n">
         <v>96</v>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G26" t="n">
         <v>0.25</v>
@@ -1591,7 +1591,7 @@
         <v>461.26</v>
       </c>
       <c r="L26" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M26" t="n">
         <v>96</v>
@@ -1617,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G27" t="n">
         <v>0.25</v>
@@ -1635,7 +1635,7 @@
         <v>461.26</v>
       </c>
       <c r="L27" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M27" t="n">
         <v>96</v>
@@ -1661,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="F28" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G28" t="n">
         <v>0.25</v>
@@ -1679,7 +1679,7 @@
         <v>410.94</v>
       </c>
       <c r="L28" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M28" t="n">
         <v>90</v>
@@ -1705,7 +1705,7 @@
         <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G29" t="n">
         <v>0.25</v>
@@ -1723,7 +1723,7 @@
         <v>410.94</v>
       </c>
       <c r="L29" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M29" t="n">
         <v>90</v>
@@ -1749,7 +1749,7 @@
         <v>100</v>
       </c>
       <c r="F30" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G30" t="n">
         <v>0.25</v>
@@ -1767,7 +1767,7 @@
         <v>179.5</v>
       </c>
       <c r="L30" t="n">
-        <v>9319720.289999999</v>
+        <v>828220.29</v>
       </c>
       <c r="M30" t="n">
         <v>37</v>
@@ -1793,7 +1793,7 @@
         <v>100</v>
       </c>
       <c r="F31" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G31" t="n">
         <v>0.25</v>
@@ -1811,7 +1811,7 @@
         <v>179.5</v>
       </c>
       <c r="L31" t="n">
-        <v>26319720.29</v>
+        <v>9319720.289999999</v>
       </c>
       <c r="M31" t="n">
         <v>37</v>
@@ -1837,7 +1837,7 @@
         <v>0.01</v>
       </c>
       <c r="F32" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G32" t="n">
         <v>0.25</v>
@@ -1855,7 +1855,7 @@
         <v>4567.6</v>
       </c>
       <c r="L32" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M32" t="n">
         <v>96</v>
@@ -1881,7 +1881,7 @@
         <v>0.01</v>
       </c>
       <c r="F33" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G33" t="n">
         <v>0.25</v>
@@ -1899,7 +1899,7 @@
         <v>4567.6</v>
       </c>
       <c r="L33" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M33" t="n">
         <v>96</v>
@@ -1925,7 +1925,7 @@
         <v>0.25</v>
       </c>
       <c r="F34" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G34" t="n">
         <v>0.25</v>
@@ -1943,7 +1943,7 @@
         <v>4566.16</v>
       </c>
       <c r="L34" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M34" t="n">
         <v>96</v>
@@ -1969,7 +1969,7 @@
         <v>0.25</v>
       </c>
       <c r="F35" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G35" t="n">
         <v>0.25</v>
@@ -1987,7 +1987,7 @@
         <v>4566.16</v>
       </c>
       <c r="L35" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M35" t="n">
         <v>96</v>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G36" t="n">
         <v>0.25</v>
@@ -2031,7 +2031,7 @@
         <v>4561.66</v>
       </c>
       <c r="L36" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M36" t="n">
         <v>96</v>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G37" t="n">
         <v>0.25</v>
@@ -2075,7 +2075,7 @@
         <v>4561.66</v>
       </c>
       <c r="L37" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M37" t="n">
         <v>96</v>
@@ -2101,7 +2101,7 @@
         <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G38" t="n">
         <v>0.25</v>
@@ -2119,7 +2119,7 @@
         <v>4509.68</v>
       </c>
       <c r="L38" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M38" t="n">
         <v>94</v>
@@ -2145,7 +2145,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G39" t="n">
         <v>0.25</v>
@@ -2163,7 +2163,7 @@
         <v>4509.68</v>
       </c>
       <c r="L39" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M39" t="n">
         <v>94</v>
@@ -2189,7 +2189,7 @@
         <v>100</v>
       </c>
       <c r="F40" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G40" t="n">
         <v>0.25</v>
@@ -2207,7 +2207,7 @@
         <v>4013.55</v>
       </c>
       <c r="L40" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M40" t="n">
         <v>89</v>
@@ -2233,7 +2233,7 @@
         <v>100</v>
       </c>
       <c r="F41" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G41" t="n">
         <v>0.25</v>
@@ -2251,7 +2251,7 @@
         <v>4013.55</v>
       </c>
       <c r="L41" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M41" t="n">
         <v>89</v>
@@ -2277,7 +2277,7 @@
         <v>0.01</v>
       </c>
       <c r="F42" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G42" t="n">
         <v>0.25</v>
@@ -2295,7 +2295,7 @@
         <v>455611.6</v>
       </c>
       <c r="L42" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M42" t="n">
         <v>96</v>
@@ -2321,7 +2321,7 @@
         <v>0.01</v>
       </c>
       <c r="F43" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G43" t="n">
         <v>0.25</v>
@@ -2339,7 +2339,7 @@
         <v>455611.6</v>
       </c>
       <c r="L43" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M43" t="n">
         <v>96</v>
@@ -2365,7 +2365,7 @@
         <v>0.25</v>
       </c>
       <c r="F44" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G44" t="n">
         <v>0.25</v>
@@ -2383,7 +2383,7 @@
         <v>455610.16</v>
       </c>
       <c r="L44" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M44" t="n">
         <v>96</v>
@@ -2409,7 +2409,7 @@
         <v>0.25</v>
       </c>
       <c r="F45" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G45" t="n">
         <v>0.25</v>
@@ -2427,7 +2427,7 @@
         <v>455610.16</v>
       </c>
       <c r="L45" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M45" t="n">
         <v>96</v>
@@ -2453,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G46" t="n">
         <v>0.25</v>
@@ -2471,7 +2471,7 @@
         <v>455605.66</v>
       </c>
       <c r="L46" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M46" t="n">
         <v>96</v>
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G47" t="n">
         <v>0.25</v>
@@ -2515,7 +2515,7 @@
         <v>455605.66</v>
       </c>
       <c r="L47" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M47" t="n">
         <v>96</v>
@@ -2541,7 +2541,7 @@
         <v>10</v>
       </c>
       <c r="F48" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G48" t="n">
         <v>0.25</v>
@@ -2559,7 +2559,7 @@
         <v>455553.68</v>
       </c>
       <c r="L48" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M48" t="n">
         <v>94</v>
@@ -2585,7 +2585,7 @@
         <v>10</v>
       </c>
       <c r="F49" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G49" t="n">
         <v>0.25</v>
@@ -2603,7 +2603,7 @@
         <v>455553.68</v>
       </c>
       <c r="L49" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M49" t="n">
         <v>94</v>
@@ -2629,7 +2629,7 @@
         <v>100</v>
       </c>
       <c r="F50" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G50" t="n">
         <v>0.25</v>
@@ -2647,7 +2647,7 @@
         <v>455034.38</v>
       </c>
       <c r="L50" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M50" t="n">
         <v>94</v>
@@ -2673,7 +2673,7 @@
         <v>100</v>
       </c>
       <c r="F51" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G51" t="n">
         <v>0.25</v>
@@ -2691,7 +2691,7 @@
         <v>455034.38</v>
       </c>
       <c r="L51" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M51" t="n">
         <v>94</v>
@@ -2717,7 +2717,7 @@
         <v>0.01</v>
       </c>
       <c r="F52" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G52" t="n">
         <v>0.25</v>
@@ -2735,7 +2735,7 @@
         <v>468.39</v>
       </c>
       <c r="L52" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M52" t="n">
         <v>97</v>
@@ -2761,7 +2761,7 @@
         <v>0.01</v>
       </c>
       <c r="F53" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G53" t="n">
         <v>0.25</v>
@@ -2779,7 +2779,7 @@
         <v>468.39</v>
       </c>
       <c r="L53" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M53" t="n">
         <v>97</v>
@@ -2805,7 +2805,7 @@
         <v>0.25</v>
       </c>
       <c r="F54" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G54" t="n">
         <v>0.25</v>
@@ -2823,7 +2823,7 @@
         <v>466.93</v>
       </c>
       <c r="L54" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M54" t="n">
         <v>97</v>
@@ -2849,7 +2849,7 @@
         <v>0.25</v>
       </c>
       <c r="F55" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G55" t="n">
         <v>0.25</v>
@@ -2867,7 +2867,7 @@
         <v>466.93</v>
       </c>
       <c r="L55" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M55" t="n">
         <v>97</v>
@@ -2893,7 +2893,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G56" t="n">
         <v>0.25</v>
@@ -2911,7 +2911,7 @@
         <v>462.36</v>
       </c>
       <c r="L56" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M56" t="n">
         <v>97</v>
@@ -2937,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G57" t="n">
         <v>0.25</v>
@@ -2955,7 +2955,7 @@
         <v>462.36</v>
       </c>
       <c r="L57" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M57" t="n">
         <v>97</v>
@@ -2981,7 +2981,7 @@
         <v>10</v>
       </c>
       <c r="F58" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G58" t="n">
         <v>0.25</v>
@@ -2999,7 +2999,7 @@
         <v>409.63</v>
       </c>
       <c r="L58" t="n">
-        <v>7069724.04</v>
+        <v>825974.04</v>
       </c>
       <c r="M58" t="n">
         <v>90</v>
@@ -3025,7 +3025,7 @@
         <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G59" t="n">
         <v>0.25</v>
@@ -3043,7 +3043,7 @@
         <v>409.63</v>
       </c>
       <c r="L59" t="n">
-        <v>19569724.04</v>
+        <v>7069724.04</v>
       </c>
       <c r="M59" t="n">
         <v>90</v>
@@ -3069,7 +3069,7 @@
         <v>100</v>
       </c>
       <c r="F60" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G60" t="n">
         <v>0.25</v>
@@ -3087,7 +3087,7 @@
         <v>117.48</v>
       </c>
       <c r="L60" t="n">
-        <v>9819720.289999999</v>
+        <v>828720.29</v>
       </c>
       <c r="M60" t="n">
         <v>45</v>
@@ -3113,7 +3113,7 @@
         <v>100</v>
       </c>
       <c r="F61" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G61" t="n">
         <v>0.25</v>
@@ -3131,7 +3131,7 @@
         <v>117.48</v>
       </c>
       <c r="L61" t="n">
-        <v>27819720.29</v>
+        <v>9819720.289999999</v>
       </c>
       <c r="M61" t="n">
         <v>45</v>
@@ -3157,7 +3157,7 @@
         <v>0.01</v>
       </c>
       <c r="F62" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G62" t="n">
         <v>0.25</v>
@@ -3175,7 +3175,7 @@
         <v>479.33</v>
       </c>
       <c r="L62" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M62" t="n">
         <v>97</v>
@@ -3201,7 +3201,7 @@
         <v>0.01</v>
       </c>
       <c r="F63" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G63" t="n">
         <v>0.25</v>
@@ -3219,7 +3219,7 @@
         <v>479.33</v>
       </c>
       <c r="L63" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M63" t="n">
         <v>97</v>
@@ -3245,7 +3245,7 @@
         <v>0.25</v>
       </c>
       <c r="F64" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G64" t="n">
         <v>0.25</v>
@@ -3263,7 +3263,7 @@
         <v>477.87</v>
       </c>
       <c r="L64" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M64" t="n">
         <v>97</v>
@@ -3289,7 +3289,7 @@
         <v>0.25</v>
       </c>
       <c r="F65" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G65" t="n">
         <v>0.25</v>
@@ -3307,7 +3307,7 @@
         <v>477.87</v>
       </c>
       <c r="L65" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M65" t="n">
         <v>97</v>
@@ -3333,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G66" t="n">
         <v>0.25</v>
@@ -3351,7 +3351,7 @@
         <v>473.29</v>
       </c>
       <c r="L66" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M66" t="n">
         <v>97</v>
@@ -3377,7 +3377,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G67" t="n">
         <v>0.25</v>
@@ -3395,7 +3395,7 @@
         <v>473.29</v>
       </c>
       <c r="L67" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M67" t="n">
         <v>97</v>
@@ -3421,7 +3421,7 @@
         <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G68" t="n">
         <v>0.25</v>
@@ -3439,7 +3439,7 @@
         <v>419.95</v>
       </c>
       <c r="L68" t="n">
-        <v>7069724.04</v>
+        <v>825974.04</v>
       </c>
       <c r="M68" t="n">
         <v>90</v>
@@ -3465,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="F69" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G69" t="n">
         <v>0.25</v>
@@ -3483,7 +3483,7 @@
         <v>419.95</v>
       </c>
       <c r="L69" t="n">
-        <v>19569724.04</v>
+        <v>7069724.04</v>
       </c>
       <c r="M69" t="n">
         <v>90</v>
@@ -3509,7 +3509,7 @@
         <v>100</v>
       </c>
       <c r="F70" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G70" t="n">
         <v>0.25</v>
@@ -3527,7 +3527,7 @@
         <v>124.25</v>
       </c>
       <c r="L70" t="n">
-        <v>9819720.289999999</v>
+        <v>828720.29</v>
       </c>
       <c r="M70" t="n">
         <v>45</v>
@@ -3553,7 +3553,7 @@
         <v>100</v>
       </c>
       <c r="F71" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G71" t="n">
         <v>0.25</v>
@@ -3571,7 +3571,7 @@
         <v>124.25</v>
       </c>
       <c r="L71" t="n">
-        <v>27819720.29</v>
+        <v>9819720.289999999</v>
       </c>
       <c r="M71" t="n">
         <v>45</v>
@@ -3597,7 +3597,7 @@
         <v>0.01</v>
       </c>
       <c r="F72" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G72" t="n">
         <v>0.25</v>
@@ -3615,7 +3615,7 @@
         <v>923.54</v>
       </c>
       <c r="L72" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M72" t="n">
         <v>97</v>
@@ -3641,7 +3641,7 @@
         <v>0.01</v>
       </c>
       <c r="F73" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G73" t="n">
         <v>0.25</v>
@@ -3659,7 +3659,7 @@
         <v>923.54</v>
       </c>
       <c r="L73" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M73" t="n">
         <v>97</v>
@@ -3685,7 +3685,7 @@
         <v>0.25</v>
       </c>
       <c r="F74" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G74" t="n">
         <v>0.25</v>
@@ -3703,7 +3703,7 @@
         <v>922.0700000000001</v>
       </c>
       <c r="L74" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M74" t="n">
         <v>97</v>
@@ -3729,7 +3729,7 @@
         <v>0.25</v>
       </c>
       <c r="F75" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G75" t="n">
         <v>0.25</v>
@@ -3747,7 +3747,7 @@
         <v>922.0700000000001</v>
       </c>
       <c r="L75" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M75" t="n">
         <v>97</v>
@@ -3773,7 +3773,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G76" t="n">
         <v>0.25</v>
@@ -3791,7 +3791,7 @@
         <v>917.5</v>
       </c>
       <c r="L76" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M76" t="n">
         <v>97</v>
@@ -3817,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G77" t="n">
         <v>0.25</v>
@@ -3835,7 +3835,7 @@
         <v>917.5</v>
       </c>
       <c r="L77" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M77" t="n">
         <v>97</v>
@@ -3861,7 +3861,7 @@
         <v>10</v>
       </c>
       <c r="F78" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G78" t="n">
         <v>0.25</v>
@@ -3879,7 +3879,7 @@
         <v>862.6</v>
       </c>
       <c r="L78" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M78" t="n">
         <v>97</v>
@@ -3905,7 +3905,7 @@
         <v>10</v>
       </c>
       <c r="F79" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G79" t="n">
         <v>0.25</v>
@@ -3923,7 +3923,7 @@
         <v>862.6</v>
       </c>
       <c r="L79" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M79" t="n">
         <v>97</v>
@@ -3949,7 +3949,7 @@
         <v>100</v>
       </c>
       <c r="F80" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G80" t="n">
         <v>0.25</v>
@@ -3967,7 +3967,7 @@
         <v>457</v>
       </c>
       <c r="L80" t="n">
-        <v>8819721.789999999</v>
+        <v>827721.79</v>
       </c>
       <c r="M80" t="n">
         <v>69</v>
@@ -3993,7 +3993,7 @@
         <v>100</v>
       </c>
       <c r="F81" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G81" t="n">
         <v>0.25</v>
@@ -4011,7 +4011,7 @@
         <v>457</v>
       </c>
       <c r="L81" t="n">
-        <v>24819721.79</v>
+        <v>8819721.789999999</v>
       </c>
       <c r="M81" t="n">
         <v>69</v>
@@ -4037,7 +4037,7 @@
         <v>0.01</v>
       </c>
       <c r="F82" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G82" t="n">
         <v>0.25</v>
@@ -4055,7 +4055,7 @@
         <v>5023.94</v>
       </c>
       <c r="L82" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M82" t="n">
         <v>97</v>
@@ -4081,7 +4081,7 @@
         <v>0.01</v>
       </c>
       <c r="F83" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G83" t="n">
         <v>0.25</v>
@@ -4099,7 +4099,7 @@
         <v>5023.94</v>
       </c>
       <c r="L83" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M83" t="n">
         <v>97</v>
@@ -4125,7 +4125,7 @@
         <v>0.25</v>
       </c>
       <c r="F84" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G84" t="n">
         <v>0.25</v>
@@ -4143,7 +4143,7 @@
         <v>5022.48</v>
       </c>
       <c r="L84" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M84" t="n">
         <v>97</v>
@@ -4169,7 +4169,7 @@
         <v>0.25</v>
       </c>
       <c r="F85" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G85" t="n">
         <v>0.25</v>
@@ -4187,7 +4187,7 @@
         <v>5022.48</v>
       </c>
       <c r="L85" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M85" t="n">
         <v>97</v>
@@ -4213,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G86" t="n">
         <v>0.25</v>
@@ -4231,7 +4231,7 @@
         <v>5017.9</v>
       </c>
       <c r="L86" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M86" t="n">
         <v>97</v>
@@ -4257,7 +4257,7 @@
         <v>1</v>
       </c>
       <c r="F87" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G87" t="n">
         <v>0.25</v>
@@ -4275,7 +4275,7 @@
         <v>5017.9</v>
       </c>
       <c r="L87" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M87" t="n">
         <v>97</v>
@@ -4301,7 +4301,7 @@
         <v>10</v>
       </c>
       <c r="F88" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G88" t="n">
         <v>0.25</v>
@@ -4319,7 +4319,7 @@
         <v>4963</v>
       </c>
       <c r="L88" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M88" t="n">
         <v>97</v>
@@ -4345,7 +4345,7 @@
         <v>10</v>
       </c>
       <c r="F89" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G89" t="n">
         <v>0.25</v>
@@ -4363,7 +4363,7 @@
         <v>4963</v>
       </c>
       <c r="L89" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M89" t="n">
         <v>97</v>
@@ -4389,7 +4389,7 @@
         <v>100</v>
       </c>
       <c r="F90" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G90" t="n">
         <v>0.25</v>
@@ -4407,7 +4407,7 @@
         <v>4437.4</v>
       </c>
       <c r="L90" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M90" t="n">
         <v>92</v>
@@ -4433,7 +4433,7 @@
         <v>100</v>
       </c>
       <c r="F91" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G91" t="n">
         <v>0.25</v>
@@ -4451,7 +4451,7 @@
         <v>4437.4</v>
       </c>
       <c r="L91" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M91" t="n">
         <v>92</v>
@@ -4477,7 +4477,7 @@
         <v>0.01</v>
       </c>
       <c r="F92" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G92" t="n">
         <v>0.25</v>
@@ -4495,7 +4495,7 @@
         <v>456066.44</v>
       </c>
       <c r="L92" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M92" t="n">
         <v>96</v>
@@ -4521,7 +4521,7 @@
         <v>0.01</v>
       </c>
       <c r="F93" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G93" t="n">
         <v>0.25</v>
@@ -4539,7 +4539,7 @@
         <v>456066.44</v>
       </c>
       <c r="L93" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M93" t="n">
         <v>96</v>
@@ -4565,7 +4565,7 @@
         <v>0.25</v>
       </c>
       <c r="F94" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G94" t="n">
         <v>0.25</v>
@@ -4583,7 +4583,7 @@
         <v>456065</v>
       </c>
       <c r="L94" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M94" t="n">
         <v>96</v>
@@ -4609,7 +4609,7 @@
         <v>0.25</v>
       </c>
       <c r="F95" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G95" t="n">
         <v>0.25</v>
@@ -4627,7 +4627,7 @@
         <v>456065</v>
       </c>
       <c r="L95" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M95" t="n">
         <v>96</v>
@@ -4653,7 +4653,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G96" t="n">
         <v>0.25</v>
@@ -4671,7 +4671,7 @@
         <v>456060.5</v>
       </c>
       <c r="L96" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M96" t="n">
         <v>96</v>
@@ -4697,7 +4697,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G97" t="n">
         <v>0.25</v>
@@ -4715,7 +4715,7 @@
         <v>456060.5</v>
       </c>
       <c r="L97" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M97" t="n">
         <v>96</v>
@@ -4741,7 +4741,7 @@
         <v>10</v>
       </c>
       <c r="F98" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G98" t="n">
         <v>0.25</v>
@@ -4759,7 +4759,7 @@
         <v>456006.5</v>
       </c>
       <c r="L98" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M98" t="n">
         <v>96</v>
@@ -4785,7 +4785,7 @@
         <v>10</v>
       </c>
       <c r="F99" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G99" t="n">
         <v>0.25</v>
@@ -4803,7 +4803,7 @@
         <v>456006.5</v>
       </c>
       <c r="L99" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M99" t="n">
         <v>96</v>
@@ -4829,7 +4829,7 @@
         <v>100</v>
       </c>
       <c r="F100" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G100" t="n">
         <v>0.25</v>
@@ -4847,7 +4847,7 @@
         <v>455478.2</v>
       </c>
       <c r="L100" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M100" t="n">
         <v>94</v>
@@ -4873,7 +4873,7 @@
         <v>100</v>
       </c>
       <c r="F101" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G101" t="n">
         <v>0.25</v>
@@ -4891,7 +4891,7 @@
         <v>455478.2</v>
       </c>
       <c r="L101" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M101" t="n">
         <v>94</v>
@@ -4917,7 +4917,7 @@
         <v>0.01</v>
       </c>
       <c r="F102" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G102" t="n">
         <v>0.25</v>
@@ -4935,7 +4935,7 @@
         <v>4680.39</v>
       </c>
       <c r="L102" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M102" t="n">
         <v>97</v>
@@ -4961,7 +4961,7 @@
         <v>0.01</v>
       </c>
       <c r="F103" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G103" t="n">
         <v>0.25</v>
@@ -4979,7 +4979,7 @@
         <v>4680.39</v>
       </c>
       <c r="L103" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M103" t="n">
         <v>97</v>
@@ -5005,7 +5005,7 @@
         <v>0.25</v>
       </c>
       <c r="F104" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G104" t="n">
         <v>0.25</v>
@@ -5023,7 +5023,7 @@
         <v>4678.93</v>
       </c>
       <c r="L104" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M104" t="n">
         <v>97</v>
@@ -5049,7 +5049,7 @@
         <v>0.25</v>
       </c>
       <c r="F105" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G105" t="n">
         <v>0.25</v>
@@ -5067,7 +5067,7 @@
         <v>4678.93</v>
       </c>
       <c r="L105" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M105" t="n">
         <v>97</v>
@@ -5093,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G106" t="n">
         <v>0.25</v>
@@ -5111,7 +5111,7 @@
         <v>4674.36</v>
       </c>
       <c r="L106" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M106" t="n">
         <v>97</v>
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G107" t="n">
         <v>0.25</v>
@@ -5155,7 +5155,7 @@
         <v>4674.36</v>
       </c>
       <c r="L107" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M107" t="n">
         <v>97</v>
@@ -5181,7 +5181,7 @@
         <v>10</v>
       </c>
       <c r="F108" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G108" t="n">
         <v>0.25</v>
@@ -5199,7 +5199,7 @@
         <v>4619.46</v>
       </c>
       <c r="L108" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M108" t="n">
         <v>97</v>
@@ -5225,7 +5225,7 @@
         <v>10</v>
       </c>
       <c r="F109" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G109" t="n">
         <v>0.25</v>
@@ -5243,7 +5243,7 @@
         <v>4619.46</v>
       </c>
       <c r="L109" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M109" t="n">
         <v>97</v>
@@ -5269,7 +5269,7 @@
         <v>100</v>
       </c>
       <c r="F110" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G110" t="n">
         <v>0.25</v>
@@ -5287,7 +5287,7 @@
         <v>4092.43</v>
       </c>
       <c r="L110" t="n">
-        <v>7069724.04</v>
+        <v>825974.04</v>
       </c>
       <c r="M110" t="n">
         <v>90</v>
@@ -5313,7 +5313,7 @@
         <v>100</v>
       </c>
       <c r="F111" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G111" t="n">
         <v>0.25</v>
@@ -5331,7 +5331,7 @@
         <v>4092.43</v>
       </c>
       <c r="L111" t="n">
-        <v>19569724.04</v>
+        <v>7069724.04</v>
       </c>
       <c r="M111" t="n">
         <v>90</v>
@@ -5357,7 +5357,7 @@
         <v>0.01</v>
       </c>
       <c r="F112" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G112" t="n">
         <v>0.25</v>
@@ -5375,7 +5375,7 @@
         <v>4691.33</v>
       </c>
       <c r="L112" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M112" t="n">
         <v>97</v>
@@ -5401,7 +5401,7 @@
         <v>0.01</v>
       </c>
       <c r="F113" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G113" t="n">
         <v>0.25</v>
@@ -5419,7 +5419,7 @@
         <v>4691.33</v>
       </c>
       <c r="L113" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M113" t="n">
         <v>97</v>
@@ -5445,7 +5445,7 @@
         <v>0.25</v>
       </c>
       <c r="F114" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G114" t="n">
         <v>0.25</v>
@@ -5463,7 +5463,7 @@
         <v>4689.87</v>
       </c>
       <c r="L114" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M114" t="n">
         <v>97</v>
@@ -5489,7 +5489,7 @@
         <v>0.25</v>
       </c>
       <c r="F115" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G115" t="n">
         <v>0.25</v>
@@ -5507,7 +5507,7 @@
         <v>4689.87</v>
       </c>
       <c r="L115" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M115" t="n">
         <v>97</v>
@@ -5533,7 +5533,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G116" t="n">
         <v>0.25</v>
@@ -5551,7 +5551,7 @@
         <v>4685.29</v>
       </c>
       <c r="L116" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M116" t="n">
         <v>97</v>
@@ -5577,7 +5577,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G117" t="n">
         <v>0.25</v>
@@ -5595,7 +5595,7 @@
         <v>4685.29</v>
       </c>
       <c r="L117" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M117" t="n">
         <v>97</v>
@@ -5621,7 +5621,7 @@
         <v>10</v>
       </c>
       <c r="F118" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G118" t="n">
         <v>0.25</v>
@@ -5639,7 +5639,7 @@
         <v>4630.39</v>
       </c>
       <c r="L118" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M118" t="n">
         <v>97</v>
@@ -5665,7 +5665,7 @@
         <v>10</v>
       </c>
       <c r="F119" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G119" t="n">
         <v>0.25</v>
@@ -5683,7 +5683,7 @@
         <v>4630.39</v>
       </c>
       <c r="L119" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M119" t="n">
         <v>97</v>
@@ -5709,7 +5709,7 @@
         <v>100</v>
       </c>
       <c r="F120" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G120" t="n">
         <v>0.25</v>
@@ -5727,7 +5727,7 @@
         <v>4102.75</v>
       </c>
       <c r="L120" t="n">
-        <v>7069724.04</v>
+        <v>825974.04</v>
       </c>
       <c r="M120" t="n">
         <v>90</v>
@@ -5753,7 +5753,7 @@
         <v>100</v>
       </c>
       <c r="F121" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G121" t="n">
         <v>0.25</v>
@@ -5771,7 +5771,7 @@
         <v>4102.75</v>
       </c>
       <c r="L121" t="n">
-        <v>19569724.04</v>
+        <v>7069724.04</v>
       </c>
       <c r="M121" t="n">
         <v>90</v>
@@ -5797,7 +5797,7 @@
         <v>0.01</v>
       </c>
       <c r="F122" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G122" t="n">
         <v>0.25</v>
@@ -5815,7 +5815,7 @@
         <v>5135.54</v>
       </c>
       <c r="L122" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M122" t="n">
         <v>97</v>
@@ -5841,7 +5841,7 @@
         <v>0.01</v>
       </c>
       <c r="F123" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G123" t="n">
         <v>0.25</v>
@@ -5859,7 +5859,7 @@
         <v>5135.54</v>
       </c>
       <c r="L123" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M123" t="n">
         <v>97</v>
@@ -5885,7 +5885,7 @@
         <v>0.25</v>
       </c>
       <c r="F124" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G124" t="n">
         <v>0.25</v>
@@ -5903,7 +5903,7 @@
         <v>5134.07</v>
       </c>
       <c r="L124" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M124" t="n">
         <v>97</v>
@@ -5929,7 +5929,7 @@
         <v>0.25</v>
       </c>
       <c r="F125" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G125" t="n">
         <v>0.25</v>
@@ -5947,7 +5947,7 @@
         <v>5134.07</v>
       </c>
       <c r="L125" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M125" t="n">
         <v>97</v>
@@ -5973,7 +5973,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G126" t="n">
         <v>0.25</v>
@@ -5991,7 +5991,7 @@
         <v>5129.5</v>
       </c>
       <c r="L126" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M126" t="n">
         <v>97</v>
@@ -6017,7 +6017,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G127" t="n">
         <v>0.25</v>
@@ -6035,7 +6035,7 @@
         <v>5129.5</v>
       </c>
       <c r="L127" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M127" t="n">
         <v>97</v>
@@ -6061,7 +6061,7 @@
         <v>10</v>
       </c>
       <c r="F128" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G128" t="n">
         <v>0.25</v>
@@ -6079,7 +6079,7 @@
         <v>5074.6</v>
       </c>
       <c r="L128" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M128" t="n">
         <v>97</v>
@@ -6105,7 +6105,7 @@
         <v>10</v>
       </c>
       <c r="F129" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G129" t="n">
         <v>0.25</v>
@@ -6123,7 +6123,7 @@
         <v>5074.6</v>
       </c>
       <c r="L129" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M129" t="n">
         <v>97</v>
@@ -6149,7 +6149,7 @@
         <v>100</v>
       </c>
       <c r="F130" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G130" t="n">
         <v>0.25</v>
@@ -6167,7 +6167,7 @@
         <v>4528.9</v>
       </c>
       <c r="L130" t="n">
-        <v>7069727.04</v>
+        <v>825977.04</v>
       </c>
       <c r="M130" t="n">
         <v>94</v>
@@ -6193,7 +6193,7 @@
         <v>100</v>
       </c>
       <c r="F131" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G131" t="n">
         <v>0.25</v>
@@ -6211,7 +6211,7 @@
         <v>4528.9</v>
       </c>
       <c r="L131" t="n">
-        <v>19569727.04</v>
+        <v>7069727.04</v>
       </c>
       <c r="M131" t="n">
         <v>94</v>
@@ -6237,7 +6237,7 @@
         <v>0.01</v>
       </c>
       <c r="F132" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G132" t="n">
         <v>0.25</v>
@@ -6255,7 +6255,7 @@
         <v>9235.940000000001</v>
       </c>
       <c r="L132" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M132" t="n">
         <v>97</v>
@@ -6281,7 +6281,7 @@
         <v>0.01</v>
       </c>
       <c r="F133" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G133" t="n">
         <v>0.25</v>
@@ -6299,7 +6299,7 @@
         <v>9235.940000000001</v>
       </c>
       <c r="L133" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M133" t="n">
         <v>97</v>
@@ -6325,7 +6325,7 @@
         <v>0.25</v>
       </c>
       <c r="F134" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G134" t="n">
         <v>0.25</v>
@@ -6343,7 +6343,7 @@
         <v>9234.48</v>
       </c>
       <c r="L134" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M134" t="n">
         <v>97</v>
@@ -6369,7 +6369,7 @@
         <v>0.25</v>
       </c>
       <c r="F135" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G135" t="n">
         <v>0.25</v>
@@ -6387,7 +6387,7 @@
         <v>9234.48</v>
       </c>
       <c r="L135" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M135" t="n">
         <v>97</v>
@@ -6413,7 +6413,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G136" t="n">
         <v>0.25</v>
@@ -6431,7 +6431,7 @@
         <v>9229.9</v>
       </c>
       <c r="L136" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M136" t="n">
         <v>97</v>
@@ -6457,7 +6457,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G137" t="n">
         <v>0.25</v>
@@ -6475,7 +6475,7 @@
         <v>9229.9</v>
       </c>
       <c r="L137" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M137" t="n">
         <v>97</v>
@@ -6501,7 +6501,7 @@
         <v>10</v>
       </c>
       <c r="F138" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G138" t="n">
         <v>0.25</v>
@@ -6519,7 +6519,7 @@
         <v>9175</v>
       </c>
       <c r="L138" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M138" t="n">
         <v>97</v>
@@ -6545,7 +6545,7 @@
         <v>10</v>
       </c>
       <c r="F139" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G139" t="n">
         <v>0.25</v>
@@ -6563,7 +6563,7 @@
         <v>9175</v>
       </c>
       <c r="L139" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M139" t="n">
         <v>97</v>
@@ -6589,7 +6589,7 @@
         <v>100</v>
       </c>
       <c r="F140" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G140" t="n">
         <v>0.25</v>
@@ -6607,7 +6607,7 @@
         <v>8626</v>
       </c>
       <c r="L140" t="n">
-        <v>7069729.29</v>
+        <v>825979.29</v>
       </c>
       <c r="M140" t="n">
         <v>97</v>
@@ -6633,7 +6633,7 @@
         <v>100</v>
       </c>
       <c r="F141" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G141" t="n">
         <v>0.25</v>
@@ -6651,7 +6651,7 @@
         <v>8626</v>
       </c>
       <c r="L141" t="n">
-        <v>19569729.29</v>
+        <v>7069729.29</v>
       </c>
       <c r="M141" t="n">
         <v>97</v>
@@ -6677,7 +6677,7 @@
         <v>0.01</v>
       </c>
       <c r="F142" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G142" t="n">
         <v>0.25</v>
@@ -6695,7 +6695,7 @@
         <v>460264.94</v>
       </c>
       <c r="L142" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M142" t="n">
         <v>96</v>
@@ -6721,7 +6721,7 @@
         <v>0.01</v>
       </c>
       <c r="F143" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G143" t="n">
         <v>0.25</v>
@@ -6739,7 +6739,7 @@
         <v>460264.94</v>
       </c>
       <c r="L143" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M143" t="n">
         <v>96</v>
@@ -6765,7 +6765,7 @@
         <v>0.25</v>
       </c>
       <c r="F144" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G144" t="n">
         <v>0.25</v>
@@ -6783,7 +6783,7 @@
         <v>460263.5</v>
       </c>
       <c r="L144" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M144" t="n">
         <v>96</v>
@@ -6809,7 +6809,7 @@
         <v>0.25</v>
       </c>
       <c r="F145" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G145" t="n">
         <v>0.25</v>
@@ -6827,7 +6827,7 @@
         <v>460263.5</v>
       </c>
       <c r="L145" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M145" t="n">
         <v>96</v>
@@ -6853,7 +6853,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G146" t="n">
         <v>0.25</v>
@@ -6871,7 +6871,7 @@
         <v>460259</v>
       </c>
       <c r="L146" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M146" t="n">
         <v>96</v>
@@ -6897,7 +6897,7 @@
         <v>1</v>
       </c>
       <c r="F147" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G147" t="n">
         <v>0.25</v>
@@ -6915,7 +6915,7 @@
         <v>460259</v>
       </c>
       <c r="L147" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M147" t="n">
         <v>96</v>
@@ -6941,7 +6941,7 @@
         <v>10</v>
       </c>
       <c r="F148" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G148" t="n">
         <v>0.25</v>
@@ -6959,7 +6959,7 @@
         <v>460205</v>
       </c>
       <c r="L148" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M148" t="n">
         <v>96</v>
@@ -6985,7 +6985,7 @@
         <v>10</v>
       </c>
       <c r="F149" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G149" t="n">
         <v>0.25</v>
@@ -7003,7 +7003,7 @@
         <v>460205</v>
       </c>
       <c r="L149" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M149" t="n">
         <v>96</v>
@@ -7029,7 +7029,7 @@
         <v>100</v>
       </c>
       <c r="F150" t="n">
-        <v>0.25</v>
+        <v>0.00025</v>
       </c>
       <c r="G150" t="n">
         <v>0.25</v>
@@ -7047,7 +7047,7 @@
         <v>459665</v>
       </c>
       <c r="L150" t="n">
-        <v>7069728.54</v>
+        <v>825978.54</v>
       </c>
       <c r="M150" t="n">
         <v>96</v>
@@ -7073,7 +7073,7 @@
         <v>100</v>
       </c>
       <c r="F151" t="n">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="G151" t="n">
         <v>0.25</v>
@@ -7091,7 +7091,7 @@
         <v>459665</v>
       </c>
       <c r="L151" t="n">
-        <v>19569728.54</v>
+        <v>7069728.54</v>
       </c>
       <c r="M151" t="n">
         <v>96</v>

</xml_diff>